<commit_message>
update 'delegation' to 'delegation preference'
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2_September.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2_September.xlsx
@@ -61,22 +61,22 @@
     <t>Trust_Rating</t>
   </si>
   <si>
-    <t>Delegation (PSAF-1/PSAF-2)</t>
-  </si>
-  <si>
-    <t>Delegation (PSAF-1/PSAF-3)</t>
-  </si>
-  <si>
-    <t>Delegation (PSAF-1/PSAF-4)</t>
-  </si>
-  <si>
-    <t>Delegation (PSAF-2/PSAF-3)</t>
-  </si>
-  <si>
-    <t>Delegation (PSAF-2/PSAF-4)</t>
-  </si>
-  <si>
-    <t>Delegation (PSAF-3/PSAF-4)</t>
+    <t>Delegation Preference (PSAF-1/PSAF-2)</t>
+  </si>
+  <si>
+    <t>Delegation Preference (PSAF-1/PSAF-3)</t>
+  </si>
+  <si>
+    <t>Delegation Preference (PSAF-1/PSAF-4)</t>
+  </si>
+  <si>
+    <t>Delegation Preference (PSAF-2/PSAF-3)</t>
+  </si>
+  <si>
+    <t>Delegation Preference (PSAF-2/PSAF-4)</t>
+  </si>
+  <si>
+    <t>Delegation Preference (PSAF-3/PSAF-4)</t>
   </si>
   <si>
     <t>Trustworthy_Rating</t>
@@ -258,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -268,9 +268,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,17 +593,17 @@
     <col min="14" max="14" style="3" width="48.86214285714286" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="3" width="23.576428571428572" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="4" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="4" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="4" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="4" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="4" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="3" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="3" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="3" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="3" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="3" width="24.005" customWidth="1" bestFit="1"/>
     <col min="22" max="22" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="23" max="23" style="3" width="17.719285714285714" customWidth="1" bestFit="1"/>
     <col min="24" max="24" style="3" width="19.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="31.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -680,7 +677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -754,7 +751,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="171.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="154.5" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -824,7 +821,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="159" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="141" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>